<commit_message>
fixed bugs in source import
</commit_message>
<xml_diff>
--- a/tests/edb/data/roads.xlsx
+++ b/tests/edb/data/roads.xlsx
@@ -460,7 +460,7 @@
     <t xml:space="preserve">tag:KOMMUNKOD</t>
   </si>
   <si>
-    <t xml:space="preserve">/home/a002469/Projects/etk/tests/edb/data/roaddata.gpkg</t>
+    <t xml:space="preserve">roaddata.gpkg</t>
   </si>
   <si>
     <t xml:space="preserve">Namn_130</t>
@@ -989,7 +989,7 @@
       <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1210,7 +1210,7 @@
       <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.69"/>
   </cols>
@@ -1493,7 +1493,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1552,7 +1552,7 @@
       <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1682,11 +1682,11 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.06"/>
@@ -1793,7 +1793,7 @@
       <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
   </cols>
@@ -1920,7 +1920,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
@@ -2094,7 +2094,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3430,7 +3430,7 @@
       <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4189,7 +4189,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4948,7 +4948,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
   </cols>
@@ -4999,7 +4999,7 @@
       <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.47"/>
   </cols>

</xml_diff>

<commit_message>
finalise export road-related sheets
</commit_message>
<xml_diff>
--- a/tests/edb/data/roads.xlsx
+++ b/tests/edb/data/roads.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="174">
   <si>
     <t xml:space="preserve">Each road (segment) has an assigned fleet and traffic situation, where the traffic situation itself can be defined by multiple attributes.</t>
   </si>
@@ -758,9 +758,6 @@
   </si>
   <si>
     <t xml:space="preserve">mg/km</t>
-  </si>
-  <si>
-    <t xml:space="preserve">import function expects same unit for all! Can force to only have unit on first row?</t>
   </si>
   <si>
     <t xml:space="preserve">description</t>
@@ -986,10 +983,10 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="I19"/>
+      <selection pane="topLeft" activeCell="I19" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1206,11 +1203,11 @@
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K3" activeCellId="0" sqref="K3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.69"/>
   </cols>
@@ -1278,9 +1275,7 @@
       <c r="J2" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>148</v>
-      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -1310,7 +1305,9 @@
       <c r="I3" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1340,7 +1337,9 @@
       <c r="I4" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J4" s="1"/>
+      <c r="J4" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -1370,7 +1369,9 @@
       <c r="I5" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1400,7 +1401,9 @@
       <c r="I6" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J6" s="1"/>
+      <c r="J6" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -1430,13 +1433,16 @@
       <c r="I7" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E9" s="4"/>
+      <c r="J9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E10" s="4"/>
@@ -1490,10 +1496,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -1503,31 +1509,31 @@
         <v>134</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>154</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1549,119 +1555,119 @@
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>161</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>163</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>68</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1682,11 +1688,11 @@
   </sheetPr>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="18.06"/>
@@ -1790,10 +1796,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.36"/>
   </cols>
@@ -1917,10 +1923,10 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="27.12"/>
@@ -2091,10 +2097,10 @@
   <dimension ref="A1:I50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -3427,10 +3433,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="topLeft" activeCell="A26" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4186,10 +4192,10 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
@@ -4945,10 +4951,10 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.16"/>
   </cols>
@@ -4996,10 +5002,10 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.47"/>
   </cols>

</xml_diff>